<commit_message>
Atualização do mês de Maio.
1 - Ajuste no cálculo do free-float das empresas;

2 - Ajuste na base de contribuição. Tabela com as contribuições t-1.
</commit_message>
<xml_diff>
--- a/bib/informes/2021/04-abril/dados/ibovespa_diario.xlsx
+++ b/bib/informes/2021/04-abril/dados/ibovespa_diario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alyss\OneDrive\Alysson\Unifor\Monitoria\indice_nupe\bib\informes\2021\04-abril\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a548da2118d25344/Alysson/Unifor/Monitoria/indice_nupe/bib/informes/2021/04-abril/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFF2A81-BB91-4C59-AB23-783E5C72894F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{3DFF2A81-BB91-4C59-AB23-783E5C72894F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF29ABB4-6BED-4BFE-BADB-973C10D47022}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,8 +55,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00%;[Red]\-0.00%"/>
+    <numFmt numFmtId="166" formatCode="0.000%"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -545,7 +546,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -557,6 +558,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -915,11 +917,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2307"/>
+  <dimension ref="A1:E2308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2286" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2287" sqref="E2287:E2306"/>
+      <pane ySplit="1" topLeftCell="A2289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2308" sqref="C2308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46889,6 +46891,12 @@
       <c r="A2307" s="1"/>
       <c r="B2307" s="2"/>
     </row>
+    <row r="2308" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2308" s="7">
+        <f>B2306/B2226 - 1</f>
+        <v>-1.0368245810439269E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <ignoredErrors>

</xml_diff>